<commit_message>
#22 add not exist type
</commit_message>
<xml_diff>
--- a/examples/milestone_5/issue_22/result.xlsx
+++ b/examples/milestone_5/issue_22/result.xlsx
@@ -183,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -206,26 +206,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,7 +556,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3"/>
@@ -929,21 +917,24 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>